<commit_message>
Piccole prove e cambi ai print
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/swap_intra_post.xlsx
+++ b/PS-VRP/Dati_output/swap_intra_post.xlsx
@@ -594,7 +594,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251164</v>
+        <v>251396</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -605,7 +605,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>156.25</v>
+        <v>35.34375</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -624,11 +624,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-07 10:14:15</t>
+          <t>2025-05-07 08:13:20</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>10000</v>
+        <v>2262</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -659,19 +659,19 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.4265625</v>
+        <v>-0.3425998263888889</v>
       </c>
       <c r="S3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251395</v>
+        <v>251164</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -682,21 +682,21 @@
         <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>35.34375</v>
+        <v>156.25</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:14:15</t>
+          <t>2025-05-07 08:13:20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:29:15</t>
+          <t>2025-05-07 08:28:20</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-07 10:29:15</t>
+          <t>2025-05-07 08:28:20</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2262</v>
+        <v>10000</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -736,19 +736,19 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
         <v>-0.4615234375</v>
       </c>
       <c r="S4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251396</v>
+        <v>251395</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
@@ -1781,7 +1781,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251743</v>
+        <v>251374</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1789,10 +1789,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D19" t="n">
-        <v>176.655737704918</v>
+        <v>448.2459016393443</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1801,21 +1801,21 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-09 07:48:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-09 07:42:00</t>
+          <t>2025-05-09 07:48:00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-09 10:38:39</t>
+          <t>2025-05-12 07:16:14</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>10776</v>
+        <v>27343</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1824,11 +1824,11 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
@@ -1841,19 +1841,19 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>244023</v>
+        <v>251743</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1861,33 +1861,33 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D20" t="n">
-        <v>16.34426229508197</v>
+        <v>176.655737704918</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-09 10:38:39</t>
+          <t>2025-05-12 07:16:14</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-09 11:07:39</t>
+          <t>2025-05-12 07:47:14</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-09 11:07:39</t>
+          <t>2025-05-12 07:47:14</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-09 11:24:00</t>
+          <t>2025-05-12 10:43:54</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>997</v>
+        <v>10776</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
@@ -1913,19 +1913,19 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2024-09-30 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-221.475</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251651</v>
+        <v>244023</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1933,33 +1933,33 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D21" t="n">
-        <v>767.7049180327868</v>
+        <v>16.34426229508197</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-09 11:24:00</t>
+          <t>2025-05-12 10:43:54</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-09 12:06:00</t>
+          <t>2025-05-12 11:12:54</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-09 12:06:00</t>
+          <t>2025-05-12 11:12:54</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-13 08:53:42</t>
+          <t>2025-05-12 11:29:14</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>46830</v>
+        <v>997</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1968,17 +1968,14 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M21" t="n">
-        <v>76</v>
-      </c>
-      <c r="N21" t="n">
-        <v>39755</v>
+        <v>70</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -1988,14 +1985,14 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2024-09-30 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.3706284153009259</v>
+        <v>-224.4786429872453</v>
       </c>
       <c r="S21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -2008,29 +2005,29 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D22" t="n">
         <v>196.7540983606557</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-13 08:53:42</t>
+          <t>2025-05-12 11:29:14</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-13 09:35:42</t>
+          <t>2025-05-12 11:54:14</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-13 09:35:42</t>
+          <t>2025-05-12 11:54:14</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-13 12:52:27</t>
+          <t>2025-05-13 07:11:00</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2064,7 +2061,7 @@
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-4.5364298725</v>
+        <v>-4.299305555555556</v>
       </c>
       <c r="S22" t="n">
         <v>1</v>
@@ -2072,7 +2069,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251374</v>
+        <v>251651</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2080,33 +2077,33 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D23" t="n">
-        <v>448.2459016393443</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-13 12:52:27</t>
+          <t>2025-05-13 07:11:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-13 13:19:27</t>
+          <t>2025-05-13 07:53:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-13 13:19:27</t>
+          <t>2025-05-13 07:53:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-14 12:47:42</t>
+          <t>2025-05-14 12:40:42</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>27343</v>
+        <v>46830</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2115,14 +2112,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M23" t="n">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="N23" t="n">
+        <v>39755</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -2132,14 +2132,14 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>0</v>
+        <v>-1.528267304189815</v>
       </c>
       <c r="S23" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -2152,29 +2152,29 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D24" t="n">
         <v>8470.786885245901</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-14 12:47:42</t>
+          <t>2025-05-14 12:40:42</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-14 13:31:42</t>
+          <t>2025-05-14 13:05:42</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-14 13:31:42</t>
+          <t>2025-05-14 13:05:42</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-06-09 10:42:29</t>
+          <t>2025-06-09 10:16:29</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2370,7 +2370,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>250894</v>
+        <v>251456</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2378,10 +2378,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D27" t="n">
-        <v>623.4084507042254</v>
+        <v>126.7464788732394</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -2390,21 +2390,21 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-08 09:49:16</t>
+          <t>2025-05-08 10:04:16</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-08 09:49:16</t>
+          <t>2025-05-08 10:04:16</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 12:12:41</t>
+          <t>2025-05-08 12:11:01</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>44262</v>
+        <v>8999</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2413,39 +2413,41 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M27" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
+        <v>39746</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>39746</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>0</v>
+        <v>-2.507658450706018</v>
       </c>
       <c r="S27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251456</v>
+        <v>244354</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2453,33 +2455,33 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D28" t="n">
-        <v>126.7464788732394</v>
+        <v>60.70422535211268</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-09 12:12:41</t>
+          <t>2025-05-08 12:11:01</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-09 12:46:41</t>
+          <t>2025-05-08 12:28:01</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-09 12:46:41</t>
+          <t>2025-05-08 12:28:01</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-09 14:53:26</t>
+          <t>2025-05-08 13:28:43</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>8999</v>
+        <v>4310</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2492,37 +2494,32 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
       </c>
-      <c r="N28" t="n">
-        <v>39746</v>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O28" t="n">
+        <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>39746</v>
+        <v>0</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>-3.620442097025463</v>
+        <v>-0.5616197183101852</v>
       </c>
       <c r="S28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251455</v>
+        <v>251547</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2530,33 +2527,33 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" t="n">
-        <v>74.6056338028169</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-09 14:53:26</t>
+          <t>2025-05-08 13:28:43</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:26</t>
+          <t>2025-05-08 13:43:43</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:10:26</t>
+          <t>2025-05-08 13:43:43</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-12 08:25:02</t>
+          <t>2025-05-09 08:48:38</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>5297</v>
+        <v>13129</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2587,11 +2584,11 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-5.350723787164352</v>
+        <v>-2.367116588414352</v>
       </c>
       <c r="S29" t="n">
         <v>7</v>
@@ -2599,7 +2596,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251547</v>
+        <v>250894</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2607,33 +2604,33 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D30" t="n">
-        <v>184.9154929577465</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-12 08:25:02</t>
+          <t>2025-05-09 08:48:38</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-12 08:40:02</t>
+          <t>2025-05-09 09:20:38</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-12 08:40:02</t>
+          <t>2025-05-09 09:20:38</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:57</t>
+          <t>2025-05-12 11:44:03</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>13129</v>
+        <v>44262</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2642,41 +2639,39 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L30" t="n">
+        <v>5</v>
+      </c>
+      <c r="M30" t="n">
+        <v>76</v>
+      </c>
+      <c r="N30" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>2025-05-05 00:00:00</t>
+        </is>
+      </c>
+      <c r="R30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
         <v>4</v>
-      </c>
-      <c r="M30" t="n">
-        <v>70</v>
-      </c>
-      <c r="N30" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P30" t="n">
-        <v>39749</v>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>2025-05-06 00:00:00</t>
-        </is>
-      </c>
-      <c r="R30" s="1" t="n">
-        <v>-5.489553990613426</v>
-      </c>
-      <c r="S30" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>244354</v>
+        <v>251455</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2684,33 +2679,33 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D31" t="n">
-        <v>60.70422535211268</v>
+        <v>74.6056338028169</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:57</t>
+          <t>2025-05-12 11:44:03</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-12 11:59:57</t>
+          <t>2025-05-12 12:16:03</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-12 11:59:57</t>
+          <t>2025-05-12 12:16:03</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-12 13:00:39</t>
+          <t>2025-05-12 13:30:39</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>4310</v>
+        <v>5297</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2728,22 +2723,27 @@
       <c r="M31" t="n">
         <v>70</v>
       </c>
-      <c r="O31" t="n">
-        <v>0</v>
+      <c r="N31" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R31" s="1" t="n">
-        <v>-4.542126369328704</v>
+        <v>-5.562959702662037</v>
       </c>
       <c r="S31" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -2763,22 +2763,22 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-12 13:00:39</t>
+          <t>2025-05-12 13:30:39</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-12 13:17:39</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-12 13:17:39</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-12 14:25:22</t>
+          <t>2025-05-12 14:55:22</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2812,7 +2812,7 @@
         </is>
       </c>
       <c r="R32" s="1" t="n">
-        <v>-19.60095852894676</v>
+        <v>-19.62179186228009</v>
       </c>
       <c r="S32" t="n">
         <v>2</v>
@@ -2835,22 +2835,22 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-12 14:25:22</t>
+          <t>2025-05-12 14:55:22</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-12 14:48:22</t>
+          <t>2025-05-13 07:18:22</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-12 14:48:22</t>
+          <t>2025-05-13 07:18:22</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-13 07:58:48</t>
+          <t>2025-05-13 08:28:48</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2884,7 +2884,7 @@
         </is>
       </c>
       <c r="R33" s="1" t="n">
-        <v>-7.332501956180556</v>
+        <v>-7.353335289513889</v>
       </c>
       <c r="S33" t="n">
         <v>2</v>
@@ -2907,22 +2907,22 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-13 07:58:48</t>
+          <t>2025-05-13 08:28:48</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-13 08:19:48</t>
+          <t>2025-05-13 08:49:48</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-13 08:19:48</t>
+          <t>2025-05-13 08:49:48</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-13 13:57:47</t>
+          <t>2025-05-13 14:27:47</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2956,7 +2956,7 @@
         </is>
       </c>
       <c r="R34" s="1" t="n">
-        <v>-8.581797730833333</v>
+        <v>-8.602631064166665</v>
       </c>
       <c r="S34" t="n">
         <v>1</v>
@@ -2979,22 +2979,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-13 13:57:47</t>
+          <t>2025-05-13 14:27:47</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-13 14:12:47</t>
+          <t>2025-05-13 14:42:47</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-13 14:12:47</t>
+          <t>2025-05-13 14:42:47</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-14 08:24:44</t>
+          <t>2025-05-14 08:54:44</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3051,22 +3051,22 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-14 08:24:44</t>
+          <t>2025-05-14 08:54:44</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-14 08:39:44</t>
+          <t>2025-05-14 09:09:44</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-14 08:39:44</t>
+          <t>2025-05-14 09:09:44</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-14 13:03:40</t>
+          <t>2025-05-14 13:33:40</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3473,7 +3473,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>251742</v>
+        <v>251626</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3481,10 +3481,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D42" t="n">
-        <v>134.8524590163935</v>
+        <v>204.9180327868852</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -3493,21 +3493,21 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 10:49:55</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>8226</v>
+        <v>12500</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3520,29 +3520,24 @@
         </is>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M42" t="n">
         <v>70</v>
       </c>
-      <c r="N42" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O42" t="n">
+        <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R42" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-8.451331967210649</v>
       </c>
       <c r="S42" t="n">
         <v>7</v>
@@ -3558,29 +3553,29 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D43" t="n">
         <v>93.67213114754098</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 10:49:55</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 11:19:55</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 11:19:55</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 12:53:35</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3619,7 +3614,7 @@
         </is>
       </c>
       <c r="R43" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-0.5372153916203704</v>
       </c>
       <c r="S43" t="n">
         <v>1</v>
@@ -3627,7 +3622,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251626</v>
+        <v>251229</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3635,33 +3630,33 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" t="n">
-        <v>204.9180327868852</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 12:53:35</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-08 13:18:35</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-08 13:18:35</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-09 07:38:26</t>
+          <t>2025-05-09 10:25:47</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>12500</v>
+        <v>18739</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3670,36 +3665,43 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M44" t="n">
         <v>70</v>
       </c>
-      <c r="O44" t="n">
-        <v>0</v>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P44" t="n">
-        <v>0</v>
+        <v>39723</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>-9.318362932604167</v>
+        <v>0</v>
       </c>
       <c r="S44" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251229</v>
+        <v>251742</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3707,33 +3709,33 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D45" t="n">
-        <v>307.1967213114754</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-09 07:38:26</t>
+          <t>2025-05-09 10:25:47</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-09 08:13:26</t>
+          <t>2025-05-09 10:55:47</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-09 08:13:26</t>
+          <t>2025-05-09 10:55:47</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-09 13:20:38</t>
+          <t>2025-05-09 13:10:38</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>18739</v>
+        <v>8226</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3742,19 +3744,17 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L45" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M45" t="n">
         <v>70</v>
       </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N45" t="n">
+        <v>39749</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
         </is>
       </c>
       <c r="P45" t="n">
-        <v>39723</v>
+        <v>39749</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
@@ -3770,10 +3770,10 @@
         </is>
       </c>
       <c r="R45" s="1" t="n">
-        <v>0</v>
+        <v>-2.549055100185185</v>
       </c>
       <c r="S45" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
@@ -3793,22 +3793,22 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-09 13:20:38</t>
+          <t>2025-05-09 13:10:38</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-09 13:45:38</t>
+          <t>2025-05-09 13:35:38</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-09 13:45:38</t>
+          <t>2025-05-09 13:35:38</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-12 10:25:52</t>
+          <t>2025-05-12 10:15:52</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3842,7 +3842,7 @@
         </is>
       </c>
       <c r="R46" s="1" t="n">
-        <v>-14.4346311475463</v>
+        <v>-14.42768670310185</v>
       </c>
       <c r="S46" t="n">
         <v>4</v>
@@ -3865,22 +3865,22 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-05-12 10:25:52</t>
+          <t>2025-05-12 10:15:52</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-12 10:50:52</t>
+          <t>2025-05-12 10:40:52</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-05-12 10:50:52</t>
+          <t>2025-05-12 10:40:52</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-05-12 13:13:10</t>
+          <t>2025-05-12 13:03:10</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3914,7 +3914,7 @@
         </is>
       </c>
       <c r="R47" s="1" t="n">
-        <v>-12.55081967212963</v>
+        <v>-12.54387522768518</v>
       </c>
       <c r="S47" t="n">
         <v>4</v>
@@ -3937,22 +3937,22 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-12 13:13:10</t>
+          <t>2025-05-12 13:03:10</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-12 13:33:10</t>
+          <t>2025-05-12 13:23:10</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-12 13:33:10</t>
+          <t>2025-05-12 13:23:10</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:29</t>
+          <t>2025-05-13 07:45:29</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4009,22 +4009,22 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:29</t>
+          <t>2025-05-13 07:45:29</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-13 08:25:29</t>
+          <t>2025-05-13 08:15:29</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-13 08:25:29</t>
+          <t>2025-05-13 08:15:29</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-13 08:37:51</t>
+          <t>2025-05-13 08:27:51</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4058,7 +4058,7 @@
         </is>
       </c>
       <c r="R49" s="1" t="n">
-        <v>-56.35961976320601</v>
+        <v>-56.35267531876157</v>
       </c>
       <c r="S49" t="n">
         <v>1</v>
@@ -4081,22 +4081,22 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-13 08:37:51</t>
+          <t>2025-05-13 08:27:51</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-13 08:57:51</t>
+          <t>2025-05-13 08:47:51</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-13 08:57:51</t>
+          <t>2025-05-13 08:47:51</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-05-14 08:19:23</t>
+          <t>2025-05-14 08:09:23</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4130,7 +4130,7 @@
         </is>
       </c>
       <c r="R50" s="1" t="n">
-        <v>-5.34680100181713</v>
+        <v>-5.339856557372685</v>
       </c>
       <c r="S50" t="n">
         <v>1</v>
@@ -4153,22 +4153,22 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-14 08:19:23</t>
+          <t>2025-05-14 08:09:23</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-14 08:39:23</t>
+          <t>2025-05-14 08:29:23</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-14 08:39:23</t>
+          <t>2025-05-14 08:29:23</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-14 09:57:23</t>
+          <t>2025-05-14 09:47:23</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4287,7 +4287,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>250923</v>
+        <v>250670</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -4295,10 +4295,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D53" t="n">
-        <v>98.67605633802818</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -4307,21 +4307,21 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-08 12:36:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-08 12:36:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-08 14:14:40</t>
+          <t>2025-05-08 12:56:00</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>7006</v>
+        <v>1563</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4330,33 +4330,28 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M53" t="n">
         <v>76</v>
       </c>
-      <c r="N53" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O53" t="n">
+        <v>0</v>
       </c>
       <c r="P53" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R53" s="1" t="n">
-        <v>-1.59352503912037</v>
+        <v>-3.538898669791666</v>
       </c>
       <c r="S53" t="n">
         <v>2</v>
@@ -4364,7 +4359,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>243569</v>
+        <v>251340</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -4375,30 +4370,30 @@
         <v>19</v>
       </c>
       <c r="D54" t="n">
-        <v>36.63380281690141</v>
+        <v>461.9718309859155</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-08 14:14:40</t>
+          <t>2025-05-08 12:56:00</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-08 14:33:40</t>
+          <t>2025-05-08 13:15:00</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-08 14:33:40</t>
+          <t>2025-05-08 13:15:00</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-09 07:10:18</t>
+          <t>2025-05-09 12:56:59</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>2601</v>
+        <v>32800</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -4407,11 +4402,11 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M54" t="n">
         <v>76</v>
@@ -4424,19 +4419,19 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>2024-09-16 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R54" s="1" t="n">
-        <v>-235.2988262910764</v>
+        <v>-11.53957355243056</v>
       </c>
       <c r="S54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>251340</v>
+        <v>243569</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -4447,30 +4442,30 @@
         <v>17</v>
       </c>
       <c r="D55" t="n">
-        <v>461.9718309859155</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-09 07:10:18</t>
+          <t>2025-05-09 12:56:59</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-09 07:27:18</t>
+          <t>2025-05-09 13:13:59</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-09 07:27:18</t>
+          <t>2025-05-09 13:13:59</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-12 07:09:16</t>
+          <t>2025-05-09 13:50:37</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>32800</v>
+        <v>2601</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4479,11 +4474,11 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M55" t="n">
         <v>76</v>
@@ -4496,14 +4491,14 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2024-09-16 00:00:00</t>
         </is>
       </c>
       <c r="R55" s="1" t="n">
-        <v>-14.29811228481481</v>
+        <v>-235.576819248831</v>
       </c>
       <c r="S55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -4516,29 +4511,29 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D56" t="n">
         <v>372.0985915492957</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-12 07:09:16</t>
+          <t>2025-05-09 13:50:37</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-12 07:39:16</t>
+          <t>2025-05-09 14:22:37</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-12 07:39:16</t>
+          <t>2025-05-09 14:22:37</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-12 13:51:22</t>
+          <t>2025-05-12 12:34:43</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4572,7 +4567,7 @@
         </is>
       </c>
       <c r="R56" s="1" t="n">
-        <v>-107.5773474178357</v>
+        <v>-107.5241099374074</v>
       </c>
       <c r="S56" t="n">
         <v>2</v>
@@ -4580,7 +4575,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>250670</v>
+        <v>250923</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -4588,33 +4583,33 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D57" t="n">
-        <v>22.01408450704225</v>
+        <v>98.67605633802818</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-12 13:51:22</t>
+          <t>2025-05-12 12:34:43</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-12 14:25:22</t>
+          <t>2025-05-12 13:10:43</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-12 14:25:22</t>
+          <t>2025-05-12 13:10:43</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-12 14:47:23</t>
+          <t>2025-05-12 14:49:23</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>1563</v>
+        <v>7006</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -4623,28 +4618,33 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L57" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M57" t="n">
         <v>76</v>
       </c>
-      <c r="O57" t="n">
-        <v>0</v>
+      <c r="N57" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P57" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-7.616246087638889</v>
+        <v>-5.617634976527778</v>
       </c>
       <c r="S57" t="n">
         <v>2</v>
@@ -4660,29 +4660,29 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D58" t="n">
         <v>464.8450704225352</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-12 14:47:23</t>
+          <t>2025-05-12 14:49:23</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:17:23</t>
+          <t>2025-05-13 07:21:23</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:17:23</t>
+          <t>2025-05-13 07:21:23</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-14 07:02:14</t>
+          <t>2025-05-14 07:06:14</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4716,7 +4716,7 @@
         </is>
       </c>
       <c r="R58" s="1" t="n">
-        <v>-285.2932218309838</v>
+        <v>-285.2959996087616</v>
       </c>
       <c r="S58" t="n">
         <v>1</v>
@@ -4739,22 +4739,22 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-14 07:02:14</t>
+          <t>2025-05-14 07:06:14</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-14 07:19:14</t>
+          <t>2025-05-14 07:23:14</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-14 07:19:14</t>
+          <t>2025-05-14 07:23:14</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-14 08:14:02</t>
+          <t>2025-05-14 08:18:02</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4811,22 +4811,22 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-14 08:14:02</t>
+          <t>2025-05-14 08:18:02</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-14 08:50:02</t>
+          <t>2025-05-14 08:54:02</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-14 08:50:02</t>
+          <t>2025-05-14 08:54:02</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-22 10:15:11</t>
+          <t>2025-05-22 10:19:11</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4868,7 +4868,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>251561</v>
+        <v>251416</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -4876,10 +4876,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D61" t="n">
-        <v>110.9183673469388</v>
+        <v>229.0204081632653</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -4888,21 +4888,21 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-08 07:50:00</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-08 07:50:00</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-08 09:40:55</t>
+          <t>2025-05-08 11:24:01</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>5435</v>
+        <v>11222</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4915,11 +4915,14 @@
         </is>
       </c>
       <c r="L61" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M61" t="n">
         <v>70</v>
       </c>
+      <c r="N61" t="n">
+        <v>39755</v>
+      </c>
       <c r="O61" t="n">
         <v>0</v>
       </c>
@@ -4928,14 +4931,14 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>2025-05-07 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R61" s="1" t="n">
-        <v>-1.403415532881944</v>
+        <v>0</v>
       </c>
       <c r="S61" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -4948,29 +4951,29 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D62" t="n">
         <v>55.44897959183673</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-08 09:40:55</t>
+          <t>2025-05-08 11:24:01</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-08 10:25:55</t>
+          <t>2025-05-08 12:04:01</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-08 10:25:55</t>
+          <t>2025-05-08 12:04:01</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-08 11:21:22</t>
+          <t>2025-05-08 12:59:28</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5004,7 +5007,7 @@
         </is>
       </c>
       <c r="R62" s="1" t="n">
-        <v>-1.473171768703704</v>
+        <v>-1.5412981859375</v>
       </c>
       <c r="S62" t="n">
         <v>8</v>
@@ -5012,7 +5015,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>251566</v>
+        <v>251561</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -5020,33 +5023,33 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D63" t="n">
-        <v>140.5918367346939</v>
+        <v>110.9183673469388</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-08 11:21:22</t>
+          <t>2025-05-08 12:59:28</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-08 12:01:22</t>
+          <t>2025-05-08 13:44:28</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-08 12:01:22</t>
+          <t>2025-05-08 13:44:28</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-08 14:21:57</t>
+          <t>2025-05-09 07:35:23</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>6889</v>
+        <v>5435</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -5059,7 +5062,7 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M63" t="n">
         <v>70</v>
@@ -5076,7 +5079,7 @@
         </is>
       </c>
       <c r="R63" s="1" t="n">
-        <v>-1.598582766435185</v>
+        <v>-2.316241496597222</v>
       </c>
       <c r="S63" t="n">
         <v>8</v>
@@ -5084,7 +5087,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>251546</v>
+        <v>251566</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -5095,30 +5098,30 @@
         <v>40</v>
       </c>
       <c r="D64" t="n">
-        <v>131.9591836734694</v>
+        <v>140.5918367346939</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-08 14:21:57</t>
+          <t>2025-05-09 07:35:23</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-09 07:01:57</t>
+          <t>2025-05-09 08:15:23</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-09 07:01:57</t>
+          <t>2025-05-09 08:15:23</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-09 09:13:55</t>
+          <t>2025-05-09 10:35:58</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>6466</v>
+        <v>6889</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5131,7 +5134,7 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M64" t="n">
         <v>70</v>
@@ -5144,19 +5147,19 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-07 00:00:00</t>
         </is>
       </c>
       <c r="R64" s="1" t="n">
-        <v>-9.384665532881945</v>
+        <v>-2.441652494328704</v>
       </c>
       <c r="S64" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>251424</v>
+        <v>251546</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -5167,30 +5170,30 @@
         <v>40</v>
       </c>
       <c r="D65" t="n">
-        <v>197.1836734693877</v>
+        <v>131.9591836734694</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-09 09:13:55</t>
+          <t>2025-05-09 10:35:58</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-09 09:53:55</t>
+          <t>2025-05-09 11:15:58</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-09 09:53:55</t>
+          <t>2025-05-09 11:15:58</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-09 13:11:06</t>
+          <t>2025-05-09 13:27:56</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>9662</v>
+        <v>6466</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -5203,7 +5206,7 @@
         </is>
       </c>
       <c r="L65" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M65" t="n">
         <v>70</v>
@@ -5216,19 +5219,19 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R65" s="1" t="n">
-        <v>-11.5493764172338</v>
+        <v>-9.561068594108797</v>
       </c>
       <c r="S65" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>251397</v>
+        <v>251424</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -5239,30 +5242,30 @@
         <v>40</v>
       </c>
       <c r="D66" t="n">
-        <v>110.9183673469388</v>
+        <v>197.1836734693877</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-09 13:11:06</t>
+          <t>2025-05-09 13:27:56</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-09 13:51:06</t>
+          <t>2025-05-09 14:07:56</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-09 13:51:06</t>
+          <t>2025-05-09 14:07:56</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-12 07:42:01</t>
+          <t>2025-05-12 09:25:07</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>5435</v>
+        <v>9662</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -5275,7 +5278,7 @@
         </is>
       </c>
       <c r="L66" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M66" t="n">
         <v>70</v>
@@ -5292,7 +5295,7 @@
         </is>
       </c>
       <c r="R66" s="1" t="n">
-        <v>-14.3208475056713</v>
+        <v>-14.39244614512732</v>
       </c>
       <c r="S66" t="n">
         <v>4</v>
@@ -5300,7 +5303,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>251416</v>
+        <v>251397</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -5311,30 +5314,30 @@
         <v>40</v>
       </c>
       <c r="D67" t="n">
-        <v>229.0204081632653</v>
+        <v>110.9183673469388</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-12 07:42:01</t>
+          <t>2025-05-12 09:25:07</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-12 08:22:01</t>
+          <t>2025-05-12 10:05:07</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-12 08:22:01</t>
+          <t>2025-05-12 10:05:07</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-12 12:11:02</t>
+          <t>2025-05-12 11:56:02</t>
         </is>
       </c>
       <c r="I67" t="n">
-        <v>11222</v>
+        <v>5435</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -5347,14 +5350,11 @@
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M67" t="n">
         <v>70</v>
       </c>
-      <c r="N67" t="n">
-        <v>39755</v>
-      </c>
       <c r="O67" t="n">
         <v>0</v>
       </c>
@@ -5363,14 +5363,14 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R67" s="1" t="n">
-        <v>0</v>
+        <v>-14.49725056689815</v>
       </c>
       <c r="S67" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68">
@@ -5383,29 +5383,29 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D68" t="n">
         <v>87.95918367346938</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-12 12:11:02</t>
+          <t>2025-05-12 11:56:02</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-12 12:56:02</t>
+          <t>2025-05-12 12:36:02</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-12 12:56:02</t>
+          <t>2025-05-12 12:36:02</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-12 14:24:00</t>
+          <t>2025-05-12 14:04:00</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5439,7 +5439,7 @@
         </is>
       </c>
       <c r="R68" s="1" t="n">
-        <v>-4.6</v>
+        <v>-4.586111111111111</v>
       </c>
       <c r="S68" t="n">
         <v>4</v>
@@ -5462,22 +5462,22 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-12 14:24:00</t>
+          <t>2025-05-12 14:04:00</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-13 07:19:00</t>
+          <t>2025-05-12 14:59:00</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-13 07:19:00</t>
+          <t>2025-05-12 14:59:00</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-13 08:37:45</t>
+          <t>2025-05-13 08:17:45</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5511,7 +5511,7 @@
         </is>
       </c>
       <c r="R69" s="1" t="n">
-        <v>-15.35955215418982</v>
+        <v>-15.34566326530093</v>
       </c>
       <c r="S69" t="n">
         <v>2</v>
@@ -5534,22 +5534,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-13 08:37:45</t>
+          <t>2025-05-13 08:17:45</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-13 09:22:45</t>
+          <t>2025-05-13 09:02:45</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-13 09:22:45</t>
+          <t>2025-05-13 09:02:45</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-13 09:38:08</t>
+          <t>2025-05-13 09:18:08</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5583,7 +5583,7 @@
         </is>
       </c>
       <c r="R70" s="1" t="n">
-        <v>-46.40148809524305</v>
+        <v>-46.38759920635417</v>
       </c>
       <c r="S70" t="n">
         <v>1</v>
@@ -5606,22 +5606,22 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-13 09:38:08</t>
+          <t>2025-05-13 09:18:08</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-13 10:23:08</t>
+          <t>2025-05-13 10:03:08</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-13 10:23:08</t>
+          <t>2025-05-13 10:03:08</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-13 12:49:07</t>
+          <t>2025-05-13 12:29:07</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5655,7 +5655,7 @@
         </is>
       </c>
       <c r="R71" s="1" t="n">
-        <v>-4.534112811793982</v>
+        <v>-4.520223922905092</v>
       </c>
       <c r="S71" t="n">
         <v>1</v>
@@ -5678,22 +5678,22 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-13 12:49:07</t>
+          <t>2025-05-13 12:29:07</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-13 13:24:07</t>
+          <t>2025-05-13 13:04:07</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-13 13:24:07</t>
+          <t>2025-05-13 13:04:07</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-14 07:50:06</t>
+          <t>2025-05-14 07:30:06</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5750,22 +5750,22 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-14 07:50:06</t>
+          <t>2025-05-14 07:30:06</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-14 08:35:06</t>
+          <t>2025-05-14 08:15:06</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-14 08:35:06</t>
+          <t>2025-05-14 08:15:06</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-14 13:42:55</t>
+          <t>2025-05-14 13:22:55</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5807,7 +5807,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>251081</v>
+        <v>251462</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -5815,10 +5815,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="D74" t="n">
-        <v>42.42253521126761</v>
+        <v>87.69014084507042</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -5827,21 +5827,21 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-09 09:07:00</t>
+          <t>2025-05-09 07:37:00</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-09 09:07:00</t>
+          <t>2025-05-09 07:37:00</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-09 09:49:25</t>
+          <t>2025-05-09 09:04:41</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>3012</v>
+        <v>6226</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -5850,38 +5850,31 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="M74" t="n">
         <v>70</v>
       </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O74" t="n">
+        <v>0</v>
       </c>
       <c r="P74" t="n">
-        <v>39750</v>
+        <v>0</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R74" s="1" t="n">
-        <v>-16.40932120501157</v>
+        <v>-0.3782570422569445</v>
       </c>
       <c r="S74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -5894,29 +5887,29 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-09 09:49:25</t>
+          <t>2025-05-09 09:04:41</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-09 12:39:41</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-09 12:39:41</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-09 12:39:41</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -5955,7 +5948,7 @@
         </is>
       </c>
       <c r="R75" s="1" t="n">
-        <v>-1.49612676056713</v>
+        <v>-1.5275625978125</v>
       </c>
       <c r="S75" t="n">
         <v>2</v>
@@ -5978,22 +5971,22 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-09 12:39:41</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-09 13:14:41</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-09 13:14:41</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-09 13:14:41</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6032,7 +6025,7 @@
         </is>
       </c>
       <c r="R76" s="1" t="n">
-        <v>-1.520432316122685</v>
+        <v>-1.551868153368056</v>
       </c>
       <c r="S76" t="n">
         <v>2</v>
@@ -6040,7 +6033,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>251594</v>
+        <v>251505</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -6048,33 +6041,33 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D77" t="n">
-        <v>91.07042253521126</v>
+        <v>200.7746478873239</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-09 13:14:41</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-12 07:54:25</t>
+          <t>2025-05-12 08:34:41</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-12 07:54:25</t>
+          <t>2025-05-12 08:34:41</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-12 09:25:29</t>
+          <t>2025-05-12 11:55:27</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>6466</v>
+        <v>14255</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -6087,7 +6080,7 @@
         </is>
       </c>
       <c r="L77" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M77" t="n">
         <v>70</v>
@@ -6100,19 +6093,19 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>2025-05-07 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R77" s="1" t="n">
-        <v>-5.392703442881944</v>
+        <v>-7.496850547731482</v>
       </c>
       <c r="S77" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>251505</v>
+        <v>251594</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -6123,30 +6116,30 @@
         <v>40</v>
       </c>
       <c r="D78" t="n">
-        <v>200.7746478873239</v>
+        <v>91.07042253521126</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-12 09:25:29</t>
+          <t>2025-05-12 11:55:27</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-12 10:05:29</t>
+          <t>2025-05-12 12:35:27</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-12 10:05:29</t>
+          <t>2025-05-12 12:35:27</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-12 13:26:16</t>
+          <t>2025-05-12 14:06:32</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>14255</v>
+        <v>6466</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
@@ -6159,7 +6152,7 @@
         </is>
       </c>
       <c r="L78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M78" t="n">
         <v>70</v>
@@ -6172,14 +6165,14 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-07 00:00:00</t>
         </is>
       </c>
       <c r="R78" s="1" t="n">
-        <v>-7.559908059467593</v>
+        <v>-5.58787167449074</v>
       </c>
       <c r="S78" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
@@ -6192,29 +6185,29 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D79" t="n">
         <v>266.5915492957747</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-12 13:26:16</t>
+          <t>2025-05-12 14:06:32</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-12 14:56:16</t>
+          <t>2025-05-13 07:41:32</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-12 14:56:16</t>
+          <t>2025-05-13 07:41:32</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-13 11:22:51</t>
+          <t>2025-05-13 12:08:07</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6248,7 +6241,7 @@
         </is>
       </c>
       <c r="R79" s="1" t="n">
-        <v>-25.47420774648148</v>
+        <v>-25.50564358372685</v>
       </c>
       <c r="S79" t="n">
         <v>2</v>
@@ -6256,7 +6249,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251462</v>
+        <v>251081</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -6264,33 +6257,33 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="D80" t="n">
-        <v>87.69014084507042</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-13 11:22:51</t>
+          <t>2025-05-13 12:08:07</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-13 13:07:51</t>
+          <t>2025-05-13 13:03:07</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-13 13:07:51</t>
+          <t>2025-05-13 13:03:07</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-13 14:35:32</t>
+          <t>2025-05-13 13:45:32</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>6226</v>
+        <v>3012</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -6299,36 +6292,43 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M80" t="n">
         <v>70</v>
       </c>
-      <c r="O80" t="n">
-        <v>0</v>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P80" t="n">
-        <v>0</v>
+        <v>39750</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R80" s="1" t="n">
-        <v>-4.608020344282407</v>
+        <v>-20.57329812206019</v>
       </c>
       <c r="S80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>250641</v>
+        <v>251466</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -6336,10 +6336,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D81" t="n">
-        <v>74.14492753623189</v>
+        <v>80.68115942028986</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -6348,21 +6348,21 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-12 07:45:00</t>
+          <t>2025-05-12 07:30:00</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-12 07:45:00</t>
+          <t>2025-05-12 07:30:00</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-12 08:59:08</t>
+          <t>2025-05-12 08:50:40</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>5116</v>
+        <v>5567</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -6375,7 +6375,7 @@
         </is>
       </c>
       <c r="L81" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M81" t="n">
         <v>70</v>
@@ -6388,19 +6388,19 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R81" s="1" t="n">
-        <v>-14.37440619967592</v>
+        <v>-3.368528582928241</v>
       </c>
       <c r="S81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>251466</v>
+        <v>250641</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -6411,30 +6411,30 @@
         <v>40</v>
       </c>
       <c r="D82" t="n">
-        <v>80.68115942028986</v>
+        <v>74.14492753623189</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-12 08:59:08</t>
+          <t>2025-05-12 08:50:40</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-05-12 09:39:08</t>
+          <t>2025-05-12 09:30:40</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-05-12 09:39:08</t>
+          <t>2025-05-12 09:30:40</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:49</t>
+          <t>2025-05-12 10:44:49</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>5567</v>
+        <v>5116</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -6447,7 +6447,7 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M82" t="n">
         <v>70</v>
@@ -6460,19 +6460,19 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R82" s="1" t="n">
-        <v>-3.458212560381945</v>
+        <v>-14.44779589371528</v>
       </c>
       <c r="S82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251465</v>
+        <v>245350</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -6480,14 +6480,14 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D83" t="n">
-        <v>90.23188405797102</v>
+        <v>405.3623188405797</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-12 10:59:49</t>
+          <t>2025-05-12 10:44:49</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6502,11 +6502,11 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-12 13:00:03</t>
+          <t>2025-05-13 10:15:11</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>6226</v>
+        <v>27970</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -6515,11 +6515,11 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M83" t="n">
         <v>70</v>
@@ -6532,19 +6532,19 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-12-31 00:00:00</t>
         </is>
       </c>
       <c r="R83" s="1" t="n">
-        <v>-3.54170692431713</v>
+        <v>0</v>
       </c>
       <c r="S83" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251557</v>
+        <v>251465</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -6552,33 +6552,33 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D84" t="n">
-        <v>97.17391304347827</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-12 13:00:03</t>
+          <t>2025-05-13 10:15:11</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-12 13:25:03</t>
+          <t>2025-05-13 11:20:11</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-12 13:25:03</t>
+          <t>2025-05-13 11:20:11</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-13 07:02:13</t>
+          <t>2025-05-13 12:50:25</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>6705</v>
+        <v>6226</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -6604,11 +6604,11 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R84" s="1" t="n">
-        <v>0</v>
+        <v>-4.535014090173611</v>
       </c>
       <c r="S84" t="n">
         <v>1</v>
@@ -6616,7 +6616,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>245350</v>
+        <v>251557</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -6624,24 +6624,24 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="D85" t="n">
-        <v>405.3623188405797</v>
+        <v>97.17391304347827</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-13 07:02:13</t>
+          <t>2025-05-13 12:50:25</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:13</t>
+          <t>2025-05-13 13:15:25</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:13</t>
+          <t>2025-05-13 13:15:25</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -6650,7 +6650,7 @@
         </is>
       </c>
       <c r="I85" t="n">
-        <v>27970</v>
+        <v>6705</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6659,11 +6659,11 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M85" t="n">
         <v>70</v>
@@ -6676,14 +6676,14 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>2025-12-31 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R85" s="1" t="n">
         <v>0</v>
       </c>
       <c r="S85" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">

</xml_diff>